<commit_message>
Bugs + constantpH and inactivationEnable (Excel>"Settings")
</commit_message>
<xml_diff>
--- a/planning/Excels/Templates/AOBNOBAMX_template.xlsx
+++ b/planning/Excels/Templates/AOBNOBAMX_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2424069M\Documents\GitHub\IbM\planning\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2424069M\Documents\GitHub\IbM\planning\Excels\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F9B15C-9AC5-4B78-8364-BA2EC2D28CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CF22CC-CD91-4419-B538-4479F49DB9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -47,10 +47,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={8FE50E6C-B28F-4752-82B4-4304353A334F}</author>
+    <author>tc={DACAAB04-91D6-46CD-8CAD-86D83E03E1FB}</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{8FE50E6C-B28F-4752-82B4-4304353A334F}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{DACAAB04-91D6-46CD-8CAD-86D83E03E1FB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -186,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="178">
   <si>
     <t>AOB/AOA</t>
   </si>
@@ -1146,6 +1146,12 @@
   <si>
     <t>[O2]=6mg/L</t>
   </si>
+  <si>
+    <t>constantpH</t>
+  </si>
+  <si>
+    <t>inacivationBac</t>
+  </si>
 </sst>
 </file>
 
@@ -1160,7 +1166,7 @@
     <numFmt numFmtId="169" formatCode="0.000"/>
     <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1404,6 +1410,12 @@
       <vertAlign val="subscript"/>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3501,7 +3513,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A2" dT="2021-11-08T19:48:53.62" personId="{5CC223E8-22CF-48C3-ABCE-0A00391E726E}" id="{8FE50E6C-B28F-4752-82B4-4304353A334F}">
+  <threadedComment ref="A2" dT="2021-11-08T19:48:53.62" personId="{5CC223E8-22CF-48C3-ABCE-0A00391E726E}" id="{DACAAB04-91D6-46CD-8CAD-86D83E03E1FB}">
     <text>only for structure_model = true</text>
   </threadedComment>
 </ThreadedComments>
@@ -3567,7 +3579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6616838C-F568-417D-8029-DEFF7E533FF8}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -7759,10 +7771,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC80DB5-92D9-44E1-984F-05E418326CA4}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7787,10 +7799,26 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="240" t="s">
+      <c r="A3" s="144" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="216" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="144" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="216" t="b">
+      <c r="B4" s="216" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="240" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="216" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7799,7 +7827,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{54BD5B48-48D3-4918-B933-84192454EDAB}">
       <formula1>"Neut,Comp,Comm,Copr"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B3" xr:uid="{E03D1A38-E4CD-4F8A-8EC3-3AE9680BF385}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B3:B5" xr:uid="{E03D1A38-E4CD-4F8A-8EC3-3AE9680BF385}">
       <formula1>"true, false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
kDist value from Excel
</commit_message>
<xml_diff>
--- a/planning/Excels/Templates/AOBNOBAMX_template.xlsx
+++ b/planning/Excels/Templates/AOBNOBAMX_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2424069M\Documents\GitHub\IbM\planning\Excels\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CF22CC-CD91-4419-B538-4479F49DB9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8A8FD5-9F52-42C4-A72A-F2803581B721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -961,9 +961,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>k</t>
-  </si>
-  <si>
     <t>s_dist</t>
   </si>
   <si>
@@ -1151,6 +1148,9 @@
   </si>
   <si>
     <t>inacivationBac</t>
+  </si>
+  <si>
+    <t>kDist</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1166,7 @@
     <numFmt numFmtId="169" formatCode="0.000"/>
     <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1410,12 +1410,6 @@
       <vertAlign val="subscript"/>
       <sz val="12"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3592,34 +3586,34 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="238" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B1" s="238" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="238" t="s">
         <v>160</v>
-      </c>
-      <c r="C1" s="238" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="237" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="88" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="C2" s="88" t="s">
         <v>172</v>
-      </c>
-      <c r="C2" s="88" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="88" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="88" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -4596,8 +4590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4714,7 +4708,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="81" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
       <c r="B9" s="224">
         <v>1</v>
@@ -4726,7 +4720,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="81" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" s="158">
         <f>2*B3</f>
@@ -4739,7 +4733,7 @@
     </row>
     <row r="11" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A11" s="146" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" s="159">
         <f>(2*B3)*0.1</f>
@@ -4799,7 +4793,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="153" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B1" s="226">
         <v>257</v>
@@ -4812,7 +4806,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="155" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="227">
         <v>257</v>
@@ -4825,7 +4819,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="155" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="228">
         <f>B5*B1</f>
@@ -4839,7 +4833,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="155" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" s="228">
         <f>B6*B2</f>
@@ -4853,7 +4847,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="155" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5" s="228">
         <f>0.000001*4</f>
@@ -4867,7 +4861,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="155" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="228">
         <f>0.000001*4</f>
@@ -4881,7 +4875,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="155" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" s="228">
         <f>0.000001*4</f>
@@ -4895,7 +4889,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="155" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B8" s="174">
         <f>5*10^(-6)</f>
@@ -4909,79 +4903,79 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="155" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B9" s="229">
         <v>5000</v>
       </c>
       <c r="C9" s="156" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" s="88"/>
       <c r="E9" s="88"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="155" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" s="228">
         <v>1E-8</v>
       </c>
       <c r="C10" s="156" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D10" s="88"/>
       <c r="E10" s="88"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="155" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B11" s="235">
         <v>0.5</v>
       </c>
       <c r="C11" s="156" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D11" s="88"/>
       <c r="E11" s="222"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="155" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B12" s="235">
         <v>0.5</v>
       </c>
       <c r="C12" s="156" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D12" s="88"/>
       <c r="E12" s="88"/>
     </row>
     <row r="13" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="172" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B13" s="236">
         <v>24</v>
       </c>
       <c r="C13" s="171" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D13" s="88"/>
       <c r="E13" s="88"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="155" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B14" s="191">
         <f>24*7</f>
         <v>168</v>
       </c>
       <c r="C14" s="234" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D14" s="88"/>
       <c r="E14" s="90"/>
@@ -5021,86 +5015,86 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="157" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B1" s="230">
         <f>1.957*10^(-9)*3600*0.7</f>
         <v>4.9316400000000006E-6</v>
       </c>
       <c r="C1" s="177" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="123" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" s="180">
         <f>1.912*10^(-9)*3600*0.7</f>
         <v>4.8182400000000001E-6</v>
       </c>
       <c r="C2" s="176" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="123" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3" s="180">
         <f>1.902*10^(-9)*3600*0.7</f>
         <v>4.7930399999999991E-6</v>
       </c>
       <c r="C3" s="176" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="123" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" s="180">
         <f>2.1*10^(-9)*3600*0.7</f>
         <v>5.2920000000000003E-6</v>
       </c>
       <c r="C4" s="176" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="123" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" s="180">
         <f>1.92*10^(-9)*3600*0.7</f>
         <v>4.8384000000000001E-6</v>
       </c>
       <c r="C5" s="176" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="123" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B6" s="180">
         <f>1.385*10^(-9)*3600*0.7</f>
         <v>3.4902000000000001E-6</v>
       </c>
       <c r="C6" s="176" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="138" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B7" s="178">
         <f>1.334*10^(-9)*3600*0.7</f>
         <v>3.3616800000000002E-6</v>
       </c>
       <c r="C7" s="179" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5121,90 +5115,90 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="181" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B1" s="231">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C1" s="154" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="182" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="221">
         <v>0.5</v>
       </c>
       <c r="C2" s="156" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="182" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" s="221">
         <v>0.5</v>
       </c>
       <c r="C3" s="156" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="182" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B4" s="221">
         <v>0.5</v>
       </c>
       <c r="C4" s="156" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="182" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" s="221">
         <v>0.5</v>
       </c>
       <c r="C5" s="156" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="182" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B6" s="221">
         <v>0.5</v>
       </c>
       <c r="C6" s="156" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="182" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="221">
         <v>0.5</v>
       </c>
       <c r="C7" s="156" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="183" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B8" s="232">
         <v>0.5</v>
       </c>
       <c r="C8" s="171" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -7773,7 +7767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC80DB5-92D9-44E1-984F-05E418326CA4}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -7784,7 +7778,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="142" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B1" s="223" t="b">
         <v>0</v>
@@ -7792,15 +7786,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="144" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" s="223" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="144" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3" s="216" t="b">
         <v>0</v>
@@ -7808,7 +7802,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="144" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" s="216" t="b">
         <v>1</v>
@@ -7816,7 +7810,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="240" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5" s="216" t="b">
         <v>1</v>
@@ -7952,7 +7946,7 @@
         <v>75</v>
       </c>
       <c r="C1" s="71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D1" s="71" t="s">
         <v>76</v>
@@ -8115,7 +8109,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="148" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B1" s="223">
         <f>(20)/(17*1000)</f>
@@ -8143,7 +8137,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="150" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="224">
         <f>8.3144/1000</f>
@@ -8157,13 +8151,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="150" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="224">
         <v>8.2057459999999999E-2</v>
       </c>
       <c r="C4" s="145" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D4" s="88"/>
       <c r="E4" s="88"/>
@@ -8183,35 +8177,35 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="150" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="180">
         <f>B7</f>
         <v>2.3271056693257722E-10</v>
       </c>
       <c r="C6" s="145" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D6" s="88"/>
       <c r="E6" s="88"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="150" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" s="180">
         <f>(((Bacteria!B8/3)*Bacteria!B1)/3)/1000</f>
         <v>2.3271056693257722E-10</v>
       </c>
       <c r="C7" s="145" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7" s="222"/>
       <c r="E7" s="88"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="150" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B8" s="233">
         <v>7.7</v>
@@ -8224,40 +8218,40 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="150" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B9" s="239">
         <v>1</v>
       </c>
       <c r="C9" s="145" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D9" s="88"/>
       <c r="E9" s="88"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="150" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" s="233">
         <v>4</v>
       </c>
       <c r="C10" s="145" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D10" s="88"/>
       <c r="E10" s="88"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="151" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B11" s="225">
         <f>(B7*1000)/0.01</f>
         <v>2.3271056693257722E-5</v>
       </c>
       <c r="C11" s="152" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D11" s="88"/>
       <c r="E11" s="88"/>

</xml_diff>